<commit_message>
Matrices de frecuencias en patrones
</commit_message>
<xml_diff>
--- a/DetectorNumeros/frecuencias/matrices_cero_10.xlsx
+++ b/DetectorNumeros/frecuencias/matrices_cero_10.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guere\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guere\Documents\Tec\7mo\IA\Programas 2do Parcial\DetectorNumeros\frecuencias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30FCBB1-DA52-4063-8203-9753B2FC440A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4ECA857-5EC0-4307-908F-C8B977509FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5232,7 +5232,7 @@
   <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC27" sqref="AC27"/>
+      <selection activeCell="AE10" sqref="AE10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>